<commit_message>
add excel comparison settings
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Financial_Sample.xlsx
+++ b/src/test/resources/excel/Financial_Sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgravi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\java-report-test-utilities\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC37B142-C915-48A1-A834-D30AF64C8D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D70B28F-17BF-4BC5-A29D-4F045E91FFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3348" yWindow="3348" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -1027,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P695"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1263,6 +1263,9 @@
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>44927</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6"/>
@@ -8865,8 +8868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D76D47-61BD-4FAC-8D3A-2E04A3E207E3}">
   <dimension ref="A1:P695"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9101,6 +9104,9 @@
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>44927</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6"/>
@@ -16703,6 +16709,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002914170AD08CD84791A27D153F5B634B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5429c1527982b506b3a2dcd5af97d528">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e53ec00ec453a1eec4584499b9bdd29">
     <xsd:element name="properties">
@@ -16816,21 +16837,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5211F8-A83C-4A0E-89EA-EB022F37C477}">
   <ds:schemaRefs>
@@ -16840,6 +16846,29 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36101D31-F691-4436-A911-BDE8158BB67A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A11FD15B-C292-4476-9AA9-A2FF2D0A22B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E22C849-2538-4665-AED1-7E13010FACF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16853,27 +16882,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A11FD15B-C292-4476-9AA9-A2FF2D0A22B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36101D31-F691-4436-A911-BDE8158BB67A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>